<commit_message>
[ADD] - More switch cases for array length
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ornella.russo\Documents\UiPath\Facturas-Dispatcher-2.0\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D092FF3-618A-47E4-B642-CBD5C760DC3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE7EF15-1475-4C61-A810-0F07084B73A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-2460" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -183,13 +183,13 @@
     <t>FacturasPath</t>
   </si>
   <si>
-    <t>C:\Users\ornella.russo\OneDrive - Softtek\Facturas Ejercicio\Facturas</t>
-  </si>
-  <si>
     <t>C:\Users\ornella.russo\OneDrive - Softtek\Facturas Ejercicio\Separadas\ORUM</t>
   </si>
   <si>
     <t>SeparadasOrumPath</t>
+  </si>
+  <si>
+    <t>C:\Users\ornella.russo\Downloads\Testing\Test</t>
   </si>
 </sst>
 </file>
@@ -557,7 +557,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -568,7 +568,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -675,15 +675,15 @@
         <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>